<commit_message>
Mejorar generacion_excel: limpiar autor, formatear mes, usar config.ini para validación de códigos
</commit_message>
<xml_diff>
--- a/generacion_excel/resultados_extraccion_noticias.xlsx
+++ b/generacion_excel/resultados_extraccion_noticias.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01/2024</t>
+          <t>Enero</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -618,7 +618,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Sí, hombre</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -628,7 +628,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -638,15 +638,15 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="O2" t="n">
-        <v>9.140000000000001</v>
+        <v>8.25</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:02</t>
+          <t>2026-01-15 11:17:21</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>02/2024</t>
+          <t>Febrero</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -727,35 +727,35 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Arola Poch</t>
+          <t>Sí, hombre</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>¿Hasta dónde puede llegar la IA en el sexo? De cumplir fantasías a modificar deseos</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>periodismo de investigación</t>
+          <t>4</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>periodismo de investigación</t>
+          <t>4</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>IA y relaciones sexuales</t>
+          <t>1</t>
         </is>
       </c>
       <c r="O3" t="n">
-        <v>7.76</v>
+        <v>7.08</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:12</t>
+          <t>2026-01-15 11:17:29</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -767,12 +767,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>María Porcel, Ver Biografía</t>
+          <t>María Porcel</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>01/2024</t>
+          <t>Enero</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -825,12 +825,12 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>María Porcel, Ver Biografía</t>
+          <t>María Porcel</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Taylor Swift</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -840,25 +840,25 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="O4" t="n">
-        <v>6.48</v>
+        <v>5.87</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:19</t>
+          <t>2026-01-15 11:17:35</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -870,12 +870,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Daniel Soufi, Ver Biografía</t>
+          <t>Daniel Soufi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01/2024</t>
+          <t>Enero</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -950,40 +950,40 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Daniel Soufi, Ver Biografía</t>
+          <t>Daniel Soufi</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Daniel Soufi</t>
+          <t>Sí, hombre</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>¿Llegaremos a hablar con los animales?</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>masculino</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>masculino</t>
+          <t>2</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>comunicacion_animal</t>
+          <t>10</t>
         </is>
       </c>
       <c r="O5" t="n">
-        <v>6.32</v>
+        <v>6.48</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:28</t>
+          <t>2026-01-15 11:17:42</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>01/2024</t>
+          <t>Enero</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Sí, hombre</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -1080,25 +1080,25 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="O6" t="n">
-        <v>7.33</v>
+        <v>6.65</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:37</t>
+          <t>2026-01-15 11:17:49</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
@@ -1110,12 +1110,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Isabel Rubio, Ver Biografía</t>
+          <t>Isabel Rubio</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>01/2024</t>
+          <t>Enero</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1178,12 +1178,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Isabel Rubio, Ver Biografía</t>
+          <t>Isabel Rubio</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>Sí</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -1203,15 +1203,15 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>15</t>
         </is>
       </c>
       <c r="O7" t="n">
-        <v>7.45</v>
+        <v>5.17</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:47</t>
+          <t>2026-01-15 11:17:55</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>04/2024</t>
+          <t>Abril</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1282,12 +1282,12 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1296,11 +1296,11 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>6.97</v>
+        <v>5.8</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>2026-01-14 12:30:55</t>
+          <t>2026-01-15 11:18:02</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06/2024</t>
+          <t>Junio</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>María De Los Ángeles Serrano Moral</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1383,12 +1383,12 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1397,11 +1397,11 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>7</v>
+        <v>4.95</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>2026-01-14 12:31:04</t>
+          <t>2026-01-15 11:18:09</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>01/2024</t>
+          <t>Enero</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1476,7 +1476,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1486,7 +1486,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1496,15 +1496,15 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>15</t>
         </is>
       </c>
       <c r="O10" t="n">
-        <v>6.97</v>
+        <v>5.82</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>2026-01-14 12:31:12</t>
+          <t>2026-01-15 11:18:16</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1516,12 +1516,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Juan José Millás, Ver Biografía</t>
+          <t>Juan José Millás</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>06/2024</t>
+          <t>Junio</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1560,40 +1560,40 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Juan José Millás, Ver Biografía</t>
+          <t>Juan José Millás</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>No aplica</t>
+          <t>2</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="O11" t="n">
-        <v>7.43</v>
+        <v>5.26</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>2026-01-14 12:31:22</t>
+          <t>2026-01-15 11:18:25</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">

</xml_diff>